<commit_message>
add events and awards pages
</commit_message>
<xml_diff>
--- a/_projects_repository/awards_table.xlsx
+++ b/_projects_repository/awards_table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/david_altare_waterboards_ca_gov/Documents/projects/water_challenge_website_test/_projects_repository/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/david_altare_waterboards_ca_gov/Documents/projects/water-data-challenge_projects-website/_projects_repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_0F66FDCE8F79A8D366075C52F35C3AB0573E8DFF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0D931C3-7F1E-4ADD-A180-A74896514F76}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_0F66FDCE8F79A8D366075C52F35C3AB0573E8DFF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37594FB2-E067-4A62-AF9B-D68B6BE1BAC3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>award_name</t>
   </si>
@@ -46,16 +46,10 @@
     <t>This award is new in 2019 and it aims to recognize the importance of scalability. The project that gets this award demonstrates impact at more than one scale and should have characteristics that reflect the success gained from iterating over multiple engagements with multiple parties at different scales.</t>
   </si>
   <si>
-    <t>Most data-licious</t>
-  </si>
-  <si>
     <t>datalicious</t>
   </si>
   <si>
     <t>This award is intended to recognize projects that effectively integrate data from different sources or organizations, including their own data.</t>
-  </si>
-  <si>
-    <t>Most engaging by design</t>
   </si>
   <si>
     <t>design</t>
@@ -91,18 +85,12 @@
     <t>This award looks at the most ambitious or highest potential for large impact as well as compelling concept and Creativity in approach.</t>
   </si>
   <si>
-    <t>People's choice</t>
-  </si>
-  <si>
     <t>peopleschoice</t>
   </si>
   <si>
     <t>This award recognizes the project that has received the most votes from the summit's in-person participants.</t>
   </si>
   <si>
-    <t>Ready to go</t>
-  </si>
-  <si>
     <t>readytogo</t>
   </si>
   <si>
@@ -118,9 +106,6 @@
     <t>This award is intended to recognize an emerging group of leaders in the water, technology, or innovation fields. The team demonstrated an innovative approach, has high leadership potential, and a diversity of organizations.</t>
   </si>
   <si>
-    <t>Team spirit and collaboration</t>
-  </si>
-  <si>
     <t>teamspirit</t>
   </si>
   <si>
@@ -131,13 +116,37 @@
   </si>
   <si>
     <t>Overall winner of the competition</t>
+  </si>
+  <si>
+    <t>Most Data-licious</t>
+  </si>
+  <si>
+    <t>Most Engaging by Design</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>Honorable Mention</t>
+  </si>
+  <si>
+    <t>People's Choice</t>
+  </si>
+  <si>
+    <t>Ready-to-Go</t>
+  </si>
+  <si>
+    <t>Runner-Up</t>
+  </si>
+  <si>
+    <t>Team Spirit and Collaboration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +158,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -523,9 +538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -563,141 +580,166 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="3" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>